<commit_message>
new add sina emai
</commit_message>
<xml_diff>
--- a/url/usefulURL.xlsx
+++ b/url/usefulURL.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3E062DD5-CB84-4CD1-9098-6D7C51132AC3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{52BB9E4D-82EA-4EE9-BFBF-B737AFE0CF91}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
   <si>
     <t>skyline</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -301,6 +301,18 @@
   </si>
   <si>
     <t>1cjy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新浪邮箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bingona@sina.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bingona1314</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -723,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1053,6 +1065,17 @@
       </c>
       <c r="C45" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C46" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1100,6 +1123,7 @@
     <hyperlink ref="B43" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
     <hyperlink ref="B44" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
     <hyperlink ref="B45" r:id="rId42" xr:uid="{9778EFE7-6B44-43AC-831A-AE14DF89768E}"/>
+    <hyperlink ref="B46" r:id="rId43" xr:uid="{F18D443F-2E48-4413-BAB3-C1E697B7465E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>